<commit_message>
Refactors UART and AT handling, restructures timer and project files
Refactors UART device structure for improved DMA handling and buffer management, enhancing AT command processing stability and memory usage. Updates timer utility, streamlines hardware abstraction, and adjusts thread stack allocations for efficiency. Removes unused linked list status code and reorganizes build/project files to support new hardware modules. Reduces heap size for optimized memory footprint.
</commit_message>
<xml_diff>
--- a/ac6demo_analysis.xlsx
+++ b/ac6demo_analysis.xlsx
@@ -116,19 +116,19 @@
     <t>thread.o</t>
   </si>
   <si>
+    <t>stm32f10x_usart.o</t>
+  </si>
+  <si>
+    <t>stm32f10x_rcc.o</t>
+  </si>
+  <si>
     <t>scanf_fp.o</t>
   </si>
   <si>
-    <t>stm32f10x_usart.o</t>
-  </si>
-  <si>
     <t>_scanf.o</t>
   </si>
   <si>
     <t>stm32f10x_adc.o</t>
-  </si>
-  <si>
-    <t>stm32f10x_rcc.o</t>
   </si>
   <si>
     <t>stm32f10x_dma.o</t>
@@ -549,85 +549,85 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="105"/>
                 <c:pt idx="0">
-                  <c:v>21.66430473327637</c:v>
+                  <c:v>24.26303863525391</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.73294258117676</c:v>
+                  <c:v>17.41496658325195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.83761978149414</c:v>
+                  <c:v>13.92290210723877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.070662498474121</c:v>
+                  <c:v>9.795918464660645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.402510643005371</c:v>
+                  <c:v>9.637187957763672</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.851387023925781</c:v>
+                  <c:v>6.553287982940674</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.462239265441895</c:v>
+                  <c:v>3.877551078796387</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.239522218704224</c:v>
+                  <c:v>3.628117799758911</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1866774559021</c:v>
+                  <c:v>2.448979616165161</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.024701356887817</c:v>
+                  <c:v>2.267573595046997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.391982197761536</c:v>
+                  <c:v>1.558956861495972</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.295808911323547</c:v>
+                  <c:v>1.451247215270996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.295808911323547</c:v>
+                  <c:v>1.451247215270996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.5669164061546326</c:v>
+                  <c:v>0.6349206566810608</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.263211190700531</c:v>
+                  <c:v>0.2947845757007599</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2227171510457993</c:v>
+                  <c:v>0.2494331002235413</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.101235069334507</c:v>
+                  <c:v>0.113378681242466</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.101235069334507</c:v>
+                  <c:v>0.113378681242466</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.08098805695772171</c:v>
+                  <c:v>0.09070295095443726</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.06074104085564613</c:v>
+                  <c:v>0.06802721321582794</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.04049402847886086</c:v>
+                  <c:v>0.04535147547721863</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.02024701423943043</c:v>
+                  <c:v>0.02267573773860931</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.02024701423943043</c:v>
+                  <c:v>0.02267573773860931</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.02024701423943043</c:v>
+                  <c:v>0.02267573773860931</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.02024701423943043</c:v>
+                  <c:v>0.02267573773860931</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.02024701423943043</c:v>
+                  <c:v>0.02267573773860931</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.005061753559857607</c:v>
+                  <c:v>0.005668934434652329</c:v>
                 </c:pt>
                 <c:pt idx="104">
                   <c:v>0</c:v>
@@ -719,16 +719,16 @@
                   <c:v>segger_rtt_printf.o</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>uart.o</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>oled_data.o</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>mf_w.l</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>oled.o</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>uart.o</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>timer.o</c:v>
@@ -737,22 +737,22 @@
                   <c:v>thread.o</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>stm32f10x_usart.o</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>stm32f10x_rcc.o</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>scanf_fp.o</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>segger_rtt.o</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>stm32f10x_usart.o</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>_scanf.o</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>stm32f10x_adc.o</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>stm32f10x_rcc.o</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>adc.o</c:v>
@@ -809,43 +809,43 @@
                   <c:v>startup_stm32f10x_md.o</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>context_rvds.o</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>stm32f10x_rtc.o</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>dmul.o</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>_scanf_str.o</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>ddiv.o</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>sys.o</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>misc.o</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>depilogue.o</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>mktime.o</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>fadd.o</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>clock.o</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>strtod.o</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>at_task.o</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>context_rvds.o</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>stm32f10x_rtc.o</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>dmul.o</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>_scanf_str.o</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>ddiv.o</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>sys.o</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>misc.o</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>depilogue.o</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>mktime.o</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>fadd.o</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>clock.o</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>strtod.o</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>localtime_i.o</c:v>
@@ -1025,316 +1025,316 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="105"/>
                 <c:pt idx="0">
-                  <c:v>13.07040119171143</c:v>
+                  <c:v>12.80328464508057</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.916547775268555</c:v>
+                  <c:v>8.128032684326172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.86891508102417</c:v>
+                  <c:v>7.708099842071533</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.811470031738281</c:v>
+                  <c:v>6.672266006469727</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.576545715332031</c:v>
+                  <c:v>4.483016014099121</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.26598072052002</c:v>
+                  <c:v>4.178798198699951</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.98209023475647</c:v>
+                  <c:v>4.010825157165527</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.806802034378052</c:v>
+                  <c:v>3.90070915222168</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.604839563369751</c:v>
+                  <c:v>3.729003429412842</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.81413745880127</c:v>
+                  <c:v>3.531168460845947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.183480978012085</c:v>
+                  <c:v>2.138857841491699</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.996760964393616</c:v>
+                  <c:v>1.955953717231751</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.672858953475952</c:v>
+                  <c:v>1.944755554199219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.627131581306458</c:v>
+                  <c:v>1.672265768051148</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.589025378227234</c:v>
+                  <c:v>1.638671159744263</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.54710865020752</c:v>
+                  <c:v>1.593878269195557</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.512813210487366</c:v>
+                  <c:v>1.515490889549255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.493760108947754</c:v>
+                  <c:v>1.481896281242371</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.482328295707703</c:v>
+                  <c:v>1.4520343542099</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.448032736778259</c:v>
+                  <c:v>1.418439745903015</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.444222211837769</c:v>
+                  <c:v>1.414706945419312</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.438506245613098</c:v>
+                  <c:v>1.40910792350769</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.383252382278442</c:v>
+                  <c:v>1.35498321056366</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.345146179199219</c:v>
+                  <c:v>1.317655801773071</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.305134773254395</c:v>
+                  <c:v>1.278462171554565</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.002191066741943</c:v>
+                  <c:v>0.9817095994949341</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.8840621113777161</c:v>
+                  <c:v>0.8659947514533997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.7849861979484558</c:v>
+                  <c:v>0.7689436078071594</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.7697437405586243</c:v>
+                  <c:v>0.7540127038955689</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.6859102845191956</c:v>
+                  <c:v>0.671892523765564</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.6516147255897522</c:v>
+                  <c:v>0.6382978558540344</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.6363722681999207</c:v>
+                  <c:v>0.6233669519424439</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.6325616836547852</c:v>
+                  <c:v>0.619634211063385</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.5677812695503235</c:v>
+                  <c:v>0.5561776757240295</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.5372963547706604</c:v>
+                  <c:v>0.5263158082962036</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.5182433128356934</c:v>
+                  <c:v>0.5076521039009094</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.4782318770885468</c:v>
+                  <c:v>0.4553937911987305</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.4648947417736054</c:v>
+                  <c:v>0.4367301166057587</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.4458416700363159</c:v>
+                  <c:v>0.4255319237709045</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.4344098269939423</c:v>
+                  <c:v>0.4180664420127869</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.4267885982990265</c:v>
+                  <c:v>0.414333701133728</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.4229779839515686</c:v>
+                  <c:v>0.3658081293106079</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.3734400272369385</c:v>
+                  <c:v>0.3620753884315491</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.3696294128894806</c:v>
+                  <c:v>0.3471444547176361</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.3543869554996491</c:v>
+                  <c:v>0.335946261882782</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.3429551422595978</c:v>
+                  <c:v>0.3284807801246643</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.335333913564682</c:v>
+                  <c:v>0.3172825574874878</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.3239020705223084</c:v>
+                  <c:v>0.3135498464107513</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.3200914561748505</c:v>
+                  <c:v>0.2874206900596619</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.2896065413951874</c:v>
+                  <c:v>0.283687949180603</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.281985342502594</c:v>
+                  <c:v>0.2762224674224854</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.2362579852342606</c:v>
+                  <c:v>0.2314296364784241</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.2133942991495132</c:v>
+                  <c:v>0.2090332210063934</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.2095836848020554</c:v>
+                  <c:v>0.2053004801273346</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.1981518566608429</c:v>
+                  <c:v>0.1941022723913193</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.1905306279659271</c:v>
+                  <c:v>0.1866368055343628</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.1905306279659271</c:v>
+                  <c:v>0.1866368055343628</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.1867200136184692</c:v>
+                  <c:v>0.182904064655304</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.1752881705760956</c:v>
+                  <c:v>0.1717058569192886</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.1638563424348831</c:v>
+                  <c:v>0.1605076491832733</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.1295608282089233</c:v>
+                  <c:v>0.1269130259752274</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.1219395995140076</c:v>
+                  <c:v>0.1194475516676903</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.1219395995140076</c:v>
+                  <c:v>0.1194475516676903</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.1181289926171303</c:v>
+                  <c:v>0.115714818239212</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.1066971495747566</c:v>
+                  <c:v>0.1045166105031967</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.1066971495747566</c:v>
+                  <c:v>0.1045166105031967</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.1028865426778793</c:v>
+                  <c:v>0.1007838770747185</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.1028865426778793</c:v>
+                  <c:v>0.1007838770747185</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.09526531398296356</c:v>
+                  <c:v>0.0933184027671814</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.09145469963550568</c:v>
+                  <c:v>0.08958566933870316</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.09145469963550568</c:v>
+                  <c:v>0.08958566933870316</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.09145469963550568</c:v>
+                  <c:v>0.08958566933870316</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.0838334783911705</c:v>
+                  <c:v>0.08212019503116608</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.07621224969625473</c:v>
+                  <c:v>0.074654720723629</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.07240163534879684</c:v>
+                  <c:v>0.07092198729515076</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.06859102845191956</c:v>
+                  <c:v>0.06718924641609192</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.06859102845191956</c:v>
+                  <c:v>0.06718924641609192</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.06859102845191956</c:v>
+                  <c:v>0.06718924641609192</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.06096979975700378</c:v>
+                  <c:v>0.05972377583384514</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.0571591891348362</c:v>
+                  <c:v>0.0559910424053669</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.0571591891348362</c:v>
+                  <c:v>0.0559910424053669</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.0571591891348362</c:v>
+                  <c:v>0.0559910424053669</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.0571591891348362</c:v>
+                  <c:v>0.0559910424053669</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.0571591891348362</c:v>
+                  <c:v>0.0559910424053669</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.05334857478737831</c:v>
+                  <c:v>0.05225830525159836</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.05334857478737831</c:v>
+                  <c:v>0.05225830525159836</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.05334857478737831</c:v>
+                  <c:v>0.05225830525159836</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.05334857478737831</c:v>
+                  <c:v>0.05225830525159836</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.04572734981775284</c:v>
+                  <c:v>0.04479283466935158</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.04572734981775284</c:v>
+                  <c:v>0.04479283466935158</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.04191673919558525</c:v>
+                  <c:v>0.04106009751558304</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.03810612484812737</c:v>
+                  <c:v>0.0373273603618145</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.03429551422595978</c:v>
+                  <c:v>0.03359462320804596</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.03429551422595978</c:v>
+                  <c:v>0.03359462320804596</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.03048489987850189</c:v>
+                  <c:v>0.02986188791692257</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.02667428739368916</c:v>
+                  <c:v>0.02612915262579918</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.02286367490887642</c:v>
+                  <c:v>0.02239641733467579</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.02286367490887642</c:v>
+                  <c:v>0.02239641733467579</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.01905306242406368</c:v>
+                  <c:v>0.01866368018090725</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.01905306242406368</c:v>
+                  <c:v>0.01866368018090725</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.01524244993925095</c:v>
+                  <c:v>0.01493094395846129</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>0.01524244993925095</c:v>
+                  <c:v>0.01493094395846129</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>0.01524244993925095</c:v>
+                  <c:v>0.01493094395846129</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>0.007621224969625473</c:v>
+                  <c:v>0.007465471979230642</c:v>
                 </c:pt>
                 <c:pt idx="104">
                   <c:v>0</c:v>
@@ -1804,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>21.66430473327637</v>
+        <v>24.26303863525391</v>
       </c>
       <c r="C3" s="1">
         <v>4280</v>
@@ -1830,10 +1830,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>20.73294258117676</v>
+        <v>17.41496658325195</v>
       </c>
       <c r="C4" s="1">
-        <v>4096</v>
+        <v>3072</v>
       </c>
       <c r="D4" s="1">
         <v>272</v>
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>4096</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1856,25 +1856,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>17.83761978149414</v>
+        <v>13.92290210723877</v>
       </c>
       <c r="C5" s="1">
-        <v>3524</v>
+        <v>2456</v>
       </c>
       <c r="D5" s="1">
-        <v>251</v>
+        <v>154</v>
       </c>
       <c r="E5" s="1">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1">
         <v>24</v>
       </c>
       <c r="H5" s="1">
-        <v>3500</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1882,10 +1882,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>9.070662498474121</v>
+        <v>9.795918464660645</v>
       </c>
       <c r="C6" s="1">
-        <v>1792</v>
+        <v>1728</v>
       </c>
       <c r="D6" s="1">
         <v>1892</v>
@@ -1900,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>1792</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1908,25 +1908,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>8.402510643005371</v>
+        <v>9.637187957763672</v>
       </c>
       <c r="C7" s="1">
-        <v>1660</v>
+        <v>1700</v>
       </c>
       <c r="D7" s="1">
-        <v>1477</v>
+        <v>2149</v>
       </c>
       <c r="E7" s="1">
-        <v>1314</v>
+        <v>1178</v>
       </c>
       <c r="F7" s="1">
         <v>43</v>
       </c>
       <c r="G7" s="1">
-        <v>120</v>
+        <v>928</v>
       </c>
       <c r="H7" s="1">
-        <v>1540</v>
+        <v>772</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1934,7 +1934,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>5.851387023925781</v>
+        <v>6.553287982940674</v>
       </c>
       <c r="C8" s="1">
         <v>1156</v>
@@ -1960,7 +1960,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>3.462239265441895</v>
+        <v>3.877551078796387</v>
       </c>
       <c r="C9" s="1">
         <v>684</v>
@@ -1986,7 +1986,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>3.239522218704224</v>
+        <v>3.628117799758911</v>
       </c>
       <c r="C10" s="1">
         <v>640</v>
@@ -2012,16 +2012,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>2.1866774559021</v>
+        <v>2.448979616165161</v>
       </c>
       <c r="C11" s="1">
         <v>432</v>
       </c>
       <c r="D11" s="1">
-        <v>4155</v>
+        <v>4355</v>
       </c>
       <c r="E11" s="1">
-        <v>2812</v>
+        <v>3012</v>
       </c>
       <c r="F11" s="1">
         <v>959</v>
@@ -2038,7 +2038,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>2.024701356887817</v>
+        <v>2.267573595046997</v>
       </c>
       <c r="C12" s="1">
         <v>400</v>
@@ -2064,7 +2064,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>1.391982197761536</v>
+        <v>1.558956861495972</v>
       </c>
       <c r="C13" s="1">
         <v>275</v>
@@ -2090,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>1.295808911323547</v>
+        <v>1.451247215270996</v>
       </c>
       <c r="C14" s="1">
         <v>256</v>
@@ -2116,7 +2116,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>1.295808911323547</v>
+        <v>1.451247215270996</v>
       </c>
       <c r="C15" s="1">
         <v>256</v>
@@ -2142,7 +2142,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>0.5669164061546326</v>
+        <v>0.6349206566810608</v>
       </c>
       <c r="C16" s="1">
         <v>112</v>
@@ -2168,7 +2168,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>0.263211190700531</v>
+        <v>0.2947845757007599</v>
       </c>
       <c r="C17" s="1">
         <v>52</v>
@@ -2194,7 +2194,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>0.2227171510457993</v>
+        <v>0.2494331002235413</v>
       </c>
       <c r="C18" s="1">
         <v>44</v>
@@ -2220,7 +2220,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>0.101235069334507</v>
+        <v>0.113378681242466</v>
       </c>
       <c r="C19" s="1">
         <v>20</v>
@@ -2246,7 +2246,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>0.101235069334507</v>
+        <v>0.113378681242466</v>
       </c>
       <c r="C20" s="1">
         <v>20</v>
@@ -2272,7 +2272,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>0.08098805695772171</v>
+        <v>0.09070295095443726</v>
       </c>
       <c r="C21" s="1">
         <v>16</v>
@@ -2298,7 +2298,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>0.06074104085564613</v>
+        <v>0.06802721321582794</v>
       </c>
       <c r="C22" s="1">
         <v>12</v>
@@ -2324,7 +2324,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>0.04049402847886086</v>
+        <v>0.04535147547721863</v>
       </c>
       <c r="C23" s="1">
         <v>8</v>
@@ -2350,7 +2350,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>0.02024701423943043</v>
+        <v>0.02267573773860931</v>
       </c>
       <c r="C24" s="1">
         <v>4</v>
@@ -2376,7 +2376,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>0.02024701423943043</v>
+        <v>0.02267573773860931</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
@@ -2402,7 +2402,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>0.02024701423943043</v>
+        <v>0.02267573773860931</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -2428,7 +2428,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>0.02024701423943043</v>
+        <v>0.02267573773860931</v>
       </c>
       <c r="C27" s="1">
         <v>4</v>
@@ -2454,7 +2454,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>0.02024701423943043</v>
+        <v>0.02267573773860931</v>
       </c>
       <c r="C28" s="1">
         <v>4</v>
@@ -2480,7 +2480,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>0.005061753559857607</v>
+        <v>0.005668934434652329</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -2590,7 +2590,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>13.07040119171143</v>
+        <v>12.80328464508057</v>
       </c>
       <c r="C3" s="1">
         <v>6860</v>
@@ -2616,16 +2616,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>7.916547775268555</v>
+        <v>8.128032684326172</v>
       </c>
       <c r="C4" s="1">
-        <v>4155</v>
+        <v>4355</v>
       </c>
       <c r="D4" s="1">
         <v>432</v>
       </c>
       <c r="E4" s="1">
-        <v>2812</v>
+        <v>3012</v>
       </c>
       <c r="F4" s="1">
         <v>959</v>
@@ -2642,7 +2642,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="2">
-        <v>7.86891508102417</v>
+        <v>7.708099842071533</v>
       </c>
       <c r="C5" s="1">
         <v>4130</v>
@@ -2668,7 +2668,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>6.811470031738281</v>
+        <v>6.672266006469727</v>
       </c>
       <c r="C6" s="1">
         <v>3575</v>
@@ -2694,7 +2694,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>4.576545715332031</v>
+        <v>4.483016014099121</v>
       </c>
       <c r="C7" s="1">
         <v>2402</v>
@@ -2720,7 +2720,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="2">
-        <v>4.26598072052002</v>
+        <v>4.178798198699951</v>
       </c>
       <c r="C8" s="1">
         <v>2239</v>
@@ -2743,48 +2743,48 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>3.98209023475647</v>
+        <v>4.010825157165527</v>
       </c>
       <c r="C9" s="1">
-        <v>2090</v>
+        <v>2149</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>1178</v>
       </c>
       <c r="F9" s="1">
-        <v>2090</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>928</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>772</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2">
-        <v>3.806802034378052</v>
+        <v>3.90070915222168</v>
       </c>
       <c r="C10" s="1">
-        <v>1998</v>
+        <v>2090</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>1998</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>2090</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -2795,54 +2795,54 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2">
-        <v>3.604839563369751</v>
+        <v>3.729003429412842</v>
       </c>
       <c r="C11" s="1">
-        <v>1892</v>
+        <v>1998</v>
       </c>
       <c r="D11" s="1">
-        <v>1792</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>1834</v>
+        <v>1998</v>
       </c>
       <c r="F11" s="1">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>1792</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>2.81413745880127</v>
+        <v>3.531168460845947</v>
       </c>
       <c r="C12" s="1">
-        <v>1477</v>
+        <v>1892</v>
       </c>
       <c r="D12" s="1">
-        <v>1660</v>
+        <v>1728</v>
       </c>
       <c r="E12" s="1">
-        <v>1314</v>
+        <v>1834</v>
       </c>
       <c r="F12" s="1">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>1540</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2850,7 +2850,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>2.183480978012085</v>
+        <v>2.138857841491699</v>
       </c>
       <c r="C13" s="1">
         <v>1146</v>
@@ -2876,7 +2876,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="2">
-        <v>1.996760964393616</v>
+        <v>1.955953717231751</v>
       </c>
       <c r="C14" s="1">
         <v>1048</v>
@@ -2902,16 +2902,16 @@
         <v>33</v>
       </c>
       <c r="B15" s="2">
-        <v>1.672858953475952</v>
+        <v>1.944755554199219</v>
       </c>
       <c r="C15" s="1">
-        <v>878</v>
+        <v>1042</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>878</v>
+        <v>1042</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2925,45 +2925,45 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2">
-        <v>1.627131581306458</v>
+        <v>1.672265768051148</v>
       </c>
       <c r="C16" s="1">
-        <v>854</v>
+        <v>896</v>
       </c>
       <c r="D16" s="1">
-        <v>4280</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>828</v>
+        <v>876</v>
       </c>
       <c r="F16" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>4280</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2">
-        <v>1.589025378227234</v>
+        <v>1.638671159744263</v>
       </c>
       <c r="C17" s="1">
-        <v>834</v>
+        <v>878</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>834</v>
+        <v>878</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -2977,28 +2977,28 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2">
-        <v>1.54710865020752</v>
+        <v>1.593878269195557</v>
       </c>
       <c r="C18" s="1">
-        <v>812</v>
+        <v>854</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
+        <v>4280</v>
       </c>
       <c r="E18" s="1">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3006,16 +3006,16 @@
         <v>36</v>
       </c>
       <c r="B19" s="2">
-        <v>1.512813210487366</v>
+        <v>1.515490889549255</v>
       </c>
       <c r="C19" s="1">
-        <v>794</v>
+        <v>812</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>794</v>
+        <v>812</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -3032,19 +3032,19 @@
         <v>37</v>
       </c>
       <c r="B20" s="2">
-        <v>1.493760108947754</v>
+        <v>1.481896281242371</v>
       </c>
       <c r="C20" s="1">
-        <v>784</v>
+        <v>794</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>764</v>
+        <v>794</v>
       </c>
       <c r="F20" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -3058,7 +3058,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="2">
-        <v>1.482328295707703</v>
+        <v>1.4520343542099</v>
       </c>
       <c r="C21" s="1">
         <v>778</v>
@@ -3084,7 +3084,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="2">
-        <v>1.448032736778259</v>
+        <v>1.418439745903015</v>
       </c>
       <c r="C22" s="1">
         <v>760</v>
@@ -3110,7 +3110,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="2">
-        <v>1.444222211837769</v>
+        <v>1.414706945419312</v>
       </c>
       <c r="C23" s="1">
         <v>758</v>
@@ -3136,7 +3136,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="2">
-        <v>1.438506245613098</v>
+        <v>1.40910792350769</v>
       </c>
       <c r="C24" s="1">
         <v>755</v>
@@ -3162,7 +3162,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="2">
-        <v>1.383252382278442</v>
+        <v>1.35498321056366</v>
       </c>
       <c r="C25" s="1">
         <v>726</v>
@@ -3188,7 +3188,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="2">
-        <v>1.345146179199219</v>
+        <v>1.317655801773071</v>
       </c>
       <c r="C26" s="1">
         <v>706</v>
@@ -3214,7 +3214,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="2">
-        <v>1.305134773254395</v>
+        <v>1.278462171554565</v>
       </c>
       <c r="C27" s="1">
         <v>685</v>
@@ -3240,7 +3240,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>1.002191066741943</v>
+        <v>0.9817095994949341</v>
       </c>
       <c r="C28" s="1">
         <v>526</v>
@@ -3266,7 +3266,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="2">
-        <v>0.8840621113777161</v>
+        <v>0.8659947514533997</v>
       </c>
       <c r="C29" s="1">
         <v>464</v>
@@ -3292,7 +3292,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="2">
-        <v>0.7849861979484558</v>
+        <v>0.7689436078071594</v>
       </c>
       <c r="C30" s="1">
         <v>412</v>
@@ -3318,7 +3318,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="2">
-        <v>0.7697437405586243</v>
+        <v>0.7540127038955689</v>
       </c>
       <c r="C31" s="1">
         <v>404</v>
@@ -3344,7 +3344,7 @@
         <v>41</v>
       </c>
       <c r="B32" s="2">
-        <v>0.6859102845191956</v>
+        <v>0.671892523765564</v>
       </c>
       <c r="C32" s="1">
         <v>360</v>
@@ -3370,7 +3370,7 @@
         <v>42</v>
       </c>
       <c r="B33" s="2">
-        <v>0.6516147255897522</v>
+        <v>0.6382978558540344</v>
       </c>
       <c r="C33" s="1">
         <v>342</v>
@@ -3396,7 +3396,7 @@
         <v>43</v>
       </c>
       <c r="B34" s="2">
-        <v>0.6363722681999207</v>
+        <v>0.6233669519424439</v>
       </c>
       <c r="C34" s="1">
         <v>334</v>
@@ -3422,7 +3422,7 @@
         <v>44</v>
       </c>
       <c r="B35" s="2">
-        <v>0.6325616836547852</v>
+        <v>0.619634211063385</v>
       </c>
       <c r="C35" s="1">
         <v>332</v>
@@ -3448,7 +3448,7 @@
         <v>25</v>
       </c>
       <c r="B36" s="2">
-        <v>0.5677812695503235</v>
+        <v>0.5561776757240295</v>
       </c>
       <c r="C36" s="1">
         <v>298</v>
@@ -3474,7 +3474,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="2">
-        <v>0.5372963547706604</v>
+        <v>0.5263158082962036</v>
       </c>
       <c r="C37" s="1">
         <v>282</v>
@@ -3500,13 +3500,13 @@
         <v>2</v>
       </c>
       <c r="B38" s="2">
-        <v>0.5182433128356934</v>
+        <v>0.5076521039009094</v>
       </c>
       <c r="C38" s="1">
         <v>272</v>
       </c>
       <c r="D38" s="1">
-        <v>4096</v>
+        <v>3072</v>
       </c>
       <c r="E38" s="1">
         <v>36</v>
@@ -3518,50 +3518,50 @@
         <v>0</v>
       </c>
       <c r="H38" s="1">
-        <v>4096</v>
+        <v>3072</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B39" s="2">
-        <v>0.4782318770885468</v>
+        <v>0.4553937911987305</v>
       </c>
       <c r="C39" s="1">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D39" s="1">
-        <v>3524</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="F39" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G39" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H39" s="1">
-        <v>3500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2">
-        <v>0.4648947417736054</v>
+        <v>0.4367301166057587</v>
       </c>
       <c r="C40" s="1">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -3575,19 +3575,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B41" s="2">
-        <v>0.4458416700363159</v>
+        <v>0.4255319237709045</v>
       </c>
       <c r="C41" s="1">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -3601,19 +3601,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B42" s="2">
-        <v>0.4344098269939423</v>
+        <v>0.4180664420127869</v>
       </c>
       <c r="C42" s="1">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -3627,19 +3627,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B43" s="2">
-        <v>0.4267885982990265</v>
+        <v>0.414333701133728</v>
       </c>
       <c r="C43" s="1">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -3653,22 +3653,22 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B44" s="2">
-        <v>0.4229779839515686</v>
+        <v>0.3658081293106079</v>
       </c>
       <c r="C44" s="1">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="F44" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
@@ -3679,22 +3679,22 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2">
-        <v>0.3734400272369385</v>
+        <v>0.3620753884315491</v>
       </c>
       <c r="C45" s="1">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F45" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
@@ -3705,19 +3705,19 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B46" s="2">
-        <v>0.3696294128894806</v>
+        <v>0.3471444547176361</v>
       </c>
       <c r="C46" s="1">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
       <c r="E46" s="1">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -3731,22 +3731,22 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B47" s="2">
-        <v>0.3543869554996491</v>
+        <v>0.335946261882782</v>
       </c>
       <c r="C47" s="1">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="F47" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -3757,22 +3757,22 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B48" s="2">
-        <v>0.3429551422595978</v>
+        <v>0.3284807801246643</v>
       </c>
       <c r="C48" s="1">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F48" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -3783,19 +3783,19 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B49" s="2">
-        <v>0.335333913564682</v>
+        <v>0.3172825574874878</v>
       </c>
       <c r="C49" s="1">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D49" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E49" s="1">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -3804,24 +3804,24 @@
         <v>0</v>
       </c>
       <c r="H49" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2">
-        <v>0.3239020705223084</v>
+        <v>0.3135498464107513</v>
       </c>
       <c r="C50" s="1">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D50" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -3830,33 +3830,33 @@
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B51" s="2">
-        <v>0.3200914561748505</v>
+        <v>0.2874206900596619</v>
       </c>
       <c r="C51" s="1">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D51" s="1">
-        <v>0</v>
+        <v>2456</v>
       </c>
       <c r="E51" s="1">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="F51" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G51" s="1">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H51" s="1">
-        <v>0</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3864,7 +3864,7 @@
         <v>56</v>
       </c>
       <c r="B52" s="2">
-        <v>0.2896065413951874</v>
+        <v>0.283687949180603</v>
       </c>
       <c r="C52" s="1">
         <v>152</v>
@@ -3890,7 +3890,7 @@
         <v>57</v>
       </c>
       <c r="B53" s="2">
-        <v>0.281985342502594</v>
+        <v>0.2762224674224854</v>
       </c>
       <c r="C53" s="1">
         <v>148</v>
@@ -3916,7 +3916,7 @@
         <v>58</v>
       </c>
       <c r="B54" s="2">
-        <v>0.2362579852342606</v>
+        <v>0.2314296364784241</v>
       </c>
       <c r="C54" s="1">
         <v>124</v>
@@ -3942,7 +3942,7 @@
         <v>59</v>
       </c>
       <c r="B55" s="2">
-        <v>0.2133942991495132</v>
+        <v>0.2090332210063934</v>
       </c>
       <c r="C55" s="1">
         <v>112</v>
@@ -3968,7 +3968,7 @@
         <v>60</v>
       </c>
       <c r="B56" s="2">
-        <v>0.2095836848020554</v>
+        <v>0.2053004801273346</v>
       </c>
       <c r="C56" s="1">
         <v>110</v>
@@ -3994,7 +3994,7 @@
         <v>61</v>
       </c>
       <c r="B57" s="2">
-        <v>0.1981518566608429</v>
+        <v>0.1941022723913193</v>
       </c>
       <c r="C57" s="1">
         <v>104</v>
@@ -4020,7 +4020,7 @@
         <v>62</v>
       </c>
       <c r="B58" s="2">
-        <v>0.1905306279659271</v>
+        <v>0.1866368055343628</v>
       </c>
       <c r="C58" s="1">
         <v>100</v>
@@ -4046,7 +4046,7 @@
         <v>63</v>
       </c>
       <c r="B59" s="2">
-        <v>0.1905306279659271</v>
+        <v>0.1866368055343628</v>
       </c>
       <c r="C59" s="1">
         <v>100</v>
@@ -4072,7 +4072,7 @@
         <v>64</v>
       </c>
       <c r="B60" s="2">
-        <v>0.1867200136184692</v>
+        <v>0.182904064655304</v>
       </c>
       <c r="C60" s="1">
         <v>98</v>
@@ -4098,7 +4098,7 @@
         <v>13</v>
       </c>
       <c r="B61" s="2">
-        <v>0.1752881705760956</v>
+        <v>0.1717058569192886</v>
       </c>
       <c r="C61" s="1">
         <v>92</v>
@@ -4124,7 +4124,7 @@
         <v>65</v>
       </c>
       <c r="B62" s="2">
-        <v>0.1638563424348831</v>
+        <v>0.1605076491832733</v>
       </c>
       <c r="C62" s="1">
         <v>86</v>
@@ -4150,7 +4150,7 @@
         <v>27</v>
       </c>
       <c r="B63" s="2">
-        <v>0.1295608282089233</v>
+        <v>0.1269130259752274</v>
       </c>
       <c r="C63" s="1">
         <v>68</v>
@@ -4176,7 +4176,7 @@
         <v>66</v>
       </c>
       <c r="B64" s="2">
-        <v>0.1219395995140076</v>
+        <v>0.1194475516676903</v>
       </c>
       <c r="C64" s="1">
         <v>64</v>
@@ -4202,7 +4202,7 @@
         <v>67</v>
       </c>
       <c r="B65" s="2">
-        <v>0.1219395995140076</v>
+        <v>0.1194475516676903</v>
       </c>
       <c r="C65" s="1">
         <v>64</v>
@@ -4228,7 +4228,7 @@
         <v>68</v>
       </c>
       <c r="B66" s="2">
-        <v>0.1181289926171303</v>
+        <v>0.115714818239212</v>
       </c>
       <c r="C66" s="1">
         <v>62</v>
@@ -4254,7 +4254,7 @@
         <v>69</v>
       </c>
       <c r="B67" s="2">
-        <v>0.1066971495747566</v>
+        <v>0.1045166105031967</v>
       </c>
       <c r="C67" s="1">
         <v>56</v>
@@ -4280,7 +4280,7 @@
         <v>70</v>
       </c>
       <c r="B68" s="2">
-        <v>0.1066971495747566</v>
+        <v>0.1045166105031967</v>
       </c>
       <c r="C68" s="1">
         <v>56</v>
@@ -4306,7 +4306,7 @@
         <v>71</v>
       </c>
       <c r="B69" s="2">
-        <v>0.1028865426778793</v>
+        <v>0.1007838770747185</v>
       </c>
       <c r="C69" s="1">
         <v>54</v>
@@ -4332,7 +4332,7 @@
         <v>72</v>
       </c>
       <c r="B70" s="2">
-        <v>0.1028865426778793</v>
+        <v>0.1007838770747185</v>
       </c>
       <c r="C70" s="1">
         <v>54</v>
@@ -4358,7 +4358,7 @@
         <v>73</v>
       </c>
       <c r="B71" s="2">
-        <v>0.09526531398296356</v>
+        <v>0.0933184027671814</v>
       </c>
       <c r="C71" s="1">
         <v>50</v>
@@ -4384,7 +4384,7 @@
         <v>74</v>
       </c>
       <c r="B72" s="2">
-        <v>0.09145469963550568</v>
+        <v>0.08958566933870316</v>
       </c>
       <c r="C72" s="1">
         <v>48</v>
@@ -4410,7 +4410,7 @@
         <v>75</v>
       </c>
       <c r="B73" s="2">
-        <v>0.09145469963550568</v>
+        <v>0.08958566933870316</v>
       </c>
       <c r="C73" s="1">
         <v>48</v>
@@ -4436,7 +4436,7 @@
         <v>76</v>
       </c>
       <c r="B74" s="2">
-        <v>0.09145469963550568</v>
+        <v>0.08958566933870316</v>
       </c>
       <c r="C74" s="1">
         <v>48</v>
@@ -4462,7 +4462,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="2">
-        <v>0.0838334783911705</v>
+        <v>0.08212019503116608</v>
       </c>
       <c r="C75" s="1">
         <v>44</v>
@@ -4488,7 +4488,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="2">
-        <v>0.07621224969625473</v>
+        <v>0.074654720723629</v>
       </c>
       <c r="C76" s="1">
         <v>40</v>
@@ -4514,7 +4514,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="2">
-        <v>0.07240163534879684</v>
+        <v>0.07092198729515076</v>
       </c>
       <c r="C77" s="1">
         <v>38</v>
@@ -4540,7 +4540,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="2">
-        <v>0.06859102845191956</v>
+        <v>0.06718924641609192</v>
       </c>
       <c r="C78" s="1">
         <v>36</v>
@@ -4566,7 +4566,7 @@
         <v>81</v>
       </c>
       <c r="B79" s="2">
-        <v>0.06859102845191956</v>
+        <v>0.06718924641609192</v>
       </c>
       <c r="C79" s="1">
         <v>36</v>
@@ -4592,7 +4592,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="2">
-        <v>0.06859102845191956</v>
+        <v>0.06718924641609192</v>
       </c>
       <c r="C80" s="1">
         <v>36</v>
@@ -4618,7 +4618,7 @@
         <v>83</v>
       </c>
       <c r="B81" s="2">
-        <v>0.06096979975700378</v>
+        <v>0.05972377583384514</v>
       </c>
       <c r="C81" s="1">
         <v>32</v>
@@ -4644,7 +4644,7 @@
         <v>84</v>
       </c>
       <c r="B82" s="2">
-        <v>0.0571591891348362</v>
+        <v>0.0559910424053669</v>
       </c>
       <c r="C82" s="1">
         <v>30</v>
@@ -4670,7 +4670,7 @@
         <v>85</v>
       </c>
       <c r="B83" s="2">
-        <v>0.0571591891348362</v>
+        <v>0.0559910424053669</v>
       </c>
       <c r="C83" s="1">
         <v>30</v>
@@ -4696,7 +4696,7 @@
         <v>86</v>
       </c>
       <c r="B84" s="2">
-        <v>0.0571591891348362</v>
+        <v>0.0559910424053669</v>
       </c>
       <c r="C84" s="1">
         <v>30</v>
@@ -4722,7 +4722,7 @@
         <v>87</v>
       </c>
       <c r="B85" s="2">
-        <v>0.0571591891348362</v>
+        <v>0.0559910424053669</v>
       </c>
       <c r="C85" s="1">
         <v>30</v>
@@ -4748,7 +4748,7 @@
         <v>55</v>
       </c>
       <c r="B86" s="2">
-        <v>0.0571591891348362</v>
+        <v>0.0559910424053669</v>
       </c>
       <c r="C86" s="1">
         <v>30</v>
@@ -4774,7 +4774,7 @@
         <v>88</v>
       </c>
       <c r="B87" s="2">
-        <v>0.05334857478737831</v>
+        <v>0.05225830525159836</v>
       </c>
       <c r="C87" s="1">
         <v>28</v>
@@ -4800,7 +4800,7 @@
         <v>89</v>
       </c>
       <c r="B88" s="2">
-        <v>0.05334857478737831</v>
+        <v>0.05225830525159836</v>
       </c>
       <c r="C88" s="1">
         <v>28</v>
@@ -4826,7 +4826,7 @@
         <v>90</v>
       </c>
       <c r="B89" s="2">
-        <v>0.05334857478737831</v>
+        <v>0.05225830525159836</v>
       </c>
       <c r="C89" s="1">
         <v>28</v>
@@ -4852,7 +4852,7 @@
         <v>91</v>
       </c>
       <c r="B90" s="2">
-        <v>0.05334857478737831</v>
+        <v>0.05225830525159836</v>
       </c>
       <c r="C90" s="1">
         <v>28</v>
@@ -4878,7 +4878,7 @@
         <v>92</v>
       </c>
       <c r="B91" s="2">
-        <v>0.04572734981775284</v>
+        <v>0.04479283466935158</v>
       </c>
       <c r="C91" s="1">
         <v>24</v>
@@ -4904,7 +4904,7 @@
         <v>93</v>
       </c>
       <c r="B92" s="2">
-        <v>0.04572734981775284</v>
+        <v>0.04479283466935158</v>
       </c>
       <c r="C92" s="1">
         <v>24</v>
@@ -4930,7 +4930,7 @@
         <v>94</v>
       </c>
       <c r="B93" s="2">
-        <v>0.04191673919558525</v>
+        <v>0.04106009751558304</v>
       </c>
       <c r="C93" s="1">
         <v>22</v>
@@ -4956,7 +4956,7 @@
         <v>95</v>
       </c>
       <c r="B94" s="2">
-        <v>0.03810612484812737</v>
+        <v>0.0373273603618145</v>
       </c>
       <c r="C94" s="1">
         <v>20</v>
@@ -4982,7 +4982,7 @@
         <v>96</v>
       </c>
       <c r="B95" s="2">
-        <v>0.03429551422595978</v>
+        <v>0.03359462320804596</v>
       </c>
       <c r="C95" s="1">
         <v>18</v>
@@ -5008,7 +5008,7 @@
         <v>97</v>
       </c>
       <c r="B96" s="2">
-        <v>0.03429551422595978</v>
+        <v>0.03359462320804596</v>
       </c>
       <c r="C96" s="1">
         <v>18</v>
@@ -5034,7 +5034,7 @@
         <v>98</v>
       </c>
       <c r="B97" s="2">
-        <v>0.03048489987850189</v>
+        <v>0.02986188791692257</v>
       </c>
       <c r="C97" s="1">
         <v>16</v>
@@ -5060,7 +5060,7 @@
         <v>99</v>
       </c>
       <c r="B98" s="2">
-        <v>0.02667428739368916</v>
+        <v>0.02612915262579918</v>
       </c>
       <c r="C98" s="1">
         <v>14</v>
@@ -5086,7 +5086,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="2">
-        <v>0.02286367490887642</v>
+        <v>0.02239641733467579</v>
       </c>
       <c r="C99" s="1">
         <v>12</v>
@@ -5112,7 +5112,7 @@
         <v>16</v>
       </c>
       <c r="B100" s="2">
-        <v>0.02286367490887642</v>
+        <v>0.02239641733467579</v>
       </c>
       <c r="C100" s="1">
         <v>12</v>
@@ -5138,7 +5138,7 @@
         <v>101</v>
       </c>
       <c r="B101" s="2">
-        <v>0.01905306242406368</v>
+        <v>0.01866368018090725</v>
       </c>
       <c r="C101" s="1">
         <v>10</v>
@@ -5164,7 +5164,7 @@
         <v>102</v>
       </c>
       <c r="B102" s="2">
-        <v>0.01905306242406368</v>
+        <v>0.01866368018090725</v>
       </c>
       <c r="C102" s="1">
         <v>10</v>
@@ -5190,7 +5190,7 @@
         <v>21</v>
       </c>
       <c r="B103" s="2">
-        <v>0.01524244993925095</v>
+        <v>0.01493094395846129</v>
       </c>
       <c r="C103" s="1">
         <v>8</v>
@@ -5216,7 +5216,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2">
-        <v>0.01524244993925095</v>
+        <v>0.01493094395846129</v>
       </c>
       <c r="C104" s="1">
         <v>8</v>
@@ -5242,7 +5242,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="2">
-        <v>0.01524244993925095</v>
+        <v>0.01493094395846129</v>
       </c>
       <c r="C105" s="1">
         <v>8</v>
@@ -5268,7 +5268,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2">
-        <v>0.007621224969625473</v>
+        <v>0.007465471979230642</v>
       </c>
       <c r="C106" s="1">
         <v>4</v>

</xml_diff>